<commit_message>
Update test data d1.xlsx: fix expected output for invalid input
</commit_message>
<xml_diff>
--- a/data/d1.xlsx
+++ b/data/d1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26960" windowHeight="9820"/>
+    <workbookView windowWidth="13800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
     <t>Monthly Pay:   $4,644.34</t>
   </si>
   <si>
-    <t>Monthly Pay:   $0.00</t>
+    <t>Please provide a positive home price value.</t>
   </si>
   <si>
     <t>false</t>
@@ -693,7 +693,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="5"/>

</xml_diff>